<commit_message>
fixed css for message when finished so it centers correctly and has white background. also tell user where files are stored
</commit_message>
<xml_diff>
--- a/sequencing/sequencing_sample_submission_forms/SamplesSubmissionForm_2016-02-18.xlsx
+++ b/sequencing/sequencing_sample_submission_forms/SamplesSubmissionForm_2016-02-18.xlsx
@@ -192,7 +192,7 @@
     <t>&lt;SAMPLE ENTRIES&gt;</t>
   </si>
   <si>
-    <t>ABX-TEP250-M-02</t>
+    <t>ABX-TEP250-M-05</t>
   </si>
   <si>
     <t>Tube</t>
@@ -213,7 +213,7 @@
     <t>250bp (HiSeq)</t>
   </si>
   <si>
-    <t>ABX-TEP251-M-02</t>
+    <t>ABX-TEP251-M-05</t>
   </si>
   <si>
     <t>air_container2</t>

</xml_diff>

<commit_message>
removed wide underline in legend
</commit_message>
<xml_diff>
--- a/sequencing/sequencing_sample_submission_forms/SamplesSubmissionForm_2016-02-18.xlsx
+++ b/sequencing/sequencing_sample_submission_forms/SamplesSubmissionForm_2016-02-18.xlsx
@@ -192,7 +192,7 @@
     <t>&lt;SAMPLE ENTRIES&gt;</t>
   </si>
   <si>
-    <t>ABX-TEP250-M-05</t>
+    <t>ABX-TEP250-M-07</t>
   </si>
   <si>
     <t>Tube</t>
@@ -213,7 +213,7 @@
     <t>250bp (HiSeq)</t>
   </si>
   <si>
-    <t>ABX-TEP251-M-05</t>
+    <t>ABX-TEP251-M-07</t>
   </si>
   <si>
     <t>air_container2</t>

</xml_diff>